<commit_message>
Get the data from excel file for the validations
</commit_message>
<xml_diff>
--- a/testdata/data.xlsx
+++ b/testdata/data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mahesh N\eclipse-workspace\ecommreplatform\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EE40E7F-AEBB-4D01-8219-48ED69EA4FC9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E90ED8DA-9954-44FF-B9D5-9FD17B244D3B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>SkuCode</t>
   </si>
@@ -55,6 +55,21 @@
   </si>
   <si>
     <t>1600</t>
+  </si>
+  <si>
+    <t>1440</t>
+  </si>
+  <si>
+    <t>TaxRate</t>
+  </si>
+  <si>
+    <t>TotalAmountIncludingTax</t>
+  </si>
+  <si>
+    <t>0.0225</t>
+  </si>
+  <si>
+    <t>1472</t>
   </si>
 </sst>
 </file>
@@ -92,7 +107,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -100,15 +115,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -423,43 +455,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F160A666-F593-447C-9349-48A911EC9325}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="3"/>
+    <col min="2" max="2" width="9.140625" style="1"/>
     <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.140625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="4" t="s">
         <v>5</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>